<commit_message>
Included groundwater flow in COMSOL model
</commit_message>
<xml_diff>
--- a/results_v4.xlsx
+++ b/results_v4.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +482,204 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B-30</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>150</v>
+      </c>
+      <c r="D3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" t="n">
+        <v>15.35860333660845</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B-39</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>150</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.1984467046723</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B-48</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>150</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11.67311575022249</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B-63</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>150</v>
+      </c>
+      <c r="D6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12.21065474546192</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B-13</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>150</v>
+      </c>
+      <c r="D7" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11.66818684759706</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B-56</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>150</v>
+      </c>
+      <c r="D8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" t="n">
+        <v>11.72986436997653</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B-179</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>150</v>
+      </c>
+      <c r="D9" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" t="n">
+        <v>11.5072466797277</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>B-180</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>150</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="n">
+        <v>11.50356061438601</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>B-21</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>300</v>
+      </c>
+      <c r="D11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" t="n">
+        <v>36.50135474911401</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>